<commit_message>
Minimal Code Docs sheets
</commit_message>
<xml_diff>
--- a/tests/xl/many-charts.xlsx
+++ b/tests/xl/many-charts.xlsx
@@ -30,10 +30,10 @@
     <t>name</t>
   </si>
   <si>
-    <t>#Title=Sheet1 - HeaderDepth=1 - IsTransposed=False - DateTime=2024-10-04 13:00:12.417228 - SchemaUrl=None</t>
-  </si>
-  <si>
-    <t>#Title=Sheet2 - HeaderDepth=1 - IsTransposed=False - DateTime=2024-10-04 13:00:12.417566 - SchemaUrl=None</t>
+    <t>#Title=Sheet1 - HeaderDepth=1 - IsTransposed=False - DateTime=2025-09-18 09:28:30.485077 - DatamodelUrl=None</t>
+  </si>
+  <si>
+    <t>#Title=Sheet2 - HeaderDepth=1 - IsTransposed=False - DateTime=2025-09-18 09:28:30.485376 - DatamodelUrl=None</t>
   </si>
   <si>
     <t>a</t>
@@ -54,7 +54,7 @@
     <t>f</t>
   </si>
   <si>
-    <t>#Title=Sheet3 - HeaderDepth=1 - IsTransposed=False - DateTime=2024-10-04 13:00:12.419116 - SchemaUrl=None</t>
+    <t>#Title=Sheet3 - HeaderDepth=1 - IsTransposed=False - DateTime=2025-09-18 09:28:30.485579 - DatamodelUrl=None</t>
   </si>
 </sst>
 </file>

</xml_diff>